<commit_message>
Export goede kolom naam
Alle kolommen staan nu goed in de export
</commit_message>
<xml_diff>
--- a/Importexcel/wwwroot/ExportIssues.xlsx
+++ b/Importexcel/wwwroot/ExportIssues.xlsx
@@ -12,11 +12,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>ease_import_sheet</t>
   </si>
   <si>
+    <t>Gereed</t>
+  </si>
+  <si>
+    <t>Project_Code</t>
+  </si>
+  <si>
+    <t>Organisatie_Code</t>
+  </si>
+  <si>
+    <t>Input_Bron</t>
+  </si>
+  <si>
+    <t>AardId</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>Categorie</t>
+  </si>
+  <si>
+    <t>Actiehouder</t>
+  </si>
+  <si>
+    <t>Prioriteit</t>
+  </si>
+  <si>
+    <t>Kenmerk</t>
+  </si>
+  <si>
+    <t>Antwoord</t>
+  </si>
+  <si>
+    <t>Opmerking</t>
+  </si>
+  <si>
+    <t>Aangever</t>
+  </si>
+  <si>
+    <t>ManUren</t>
+  </si>
+  <si>
+    <t>Datum_Ingediend</t>
+  </si>
+  <si>
+    <t>Datum_Gepland</t>
+  </si>
+  <si>
+    <t>Datum_Gereed</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>Nee</t>
   </si>
   <si>
@@ -150,6 +207,39 @@
   </si>
   <si>
     <t>4-11-2018 00:00:00</t>
+  </si>
+  <si>
+    <t>12312</t>
+  </si>
+  <si>
+    <t>312htr</t>
+  </si>
+  <si>
+    <t>646muy</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Browser Loopt vast</t>
+  </si>
+  <si>
+    <t>Hisham</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>bekende bug , wordt opgelost</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>5-11-2018 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -195,31 +285,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.4037666320801" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.51844501495361" customWidth="1"/>
+    <col min="2" max="2" width="13.2158031463623" customWidth="1"/>
+    <col min="3" max="3" width="17.0134220123291" customWidth="1"/>
+    <col min="4" max="4" width="11.3517770767212" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="30.0002117156982" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.86935520172119" customWidth="1"/>
+    <col min="8" max="8" width="12.2316131591797" customWidth="1"/>
+    <col min="9" max="9" width="9.17571830749512" customWidth="1"/>
+    <col min="10" max="10" width="9.27290916442871" customWidth="1"/>
     <col min="11" max="11" width="30.0002117156982" customWidth="1"/>
     <col min="12" max="12" width="27.8681449890137" customWidth="1"/>
     <col min="13" max="13" width="17.1269817352295" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.7199878692627" customWidth="1"/>
+    <col min="15" max="15" width="9.7690954208374" customWidth="1"/>
     <col min="16" max="16" width="19.6877136230469" customWidth="1"/>
     <col min="17" max="17" width="19.6877136230469" customWidth="1"/>
     <col min="18" max="18" width="19.6877136230469" customWidth="1"/>
     <col min="19" max="19" width="12.547739982605" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -227,181 +318,314 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="T4" s="0">
+        <v>1048</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>34</v>
+        <v>53</v>
+      </c>
+      <c r="T5" s="0">
+        <v>1049</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>17</v>
+      <c r="T6" s="0">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" s="0">
+        <v>1051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Labels geupdate en downloaden template
Labels geupdate en downloaden template
</commit_message>
<xml_diff>
--- a/Importexcel/wwwroot/ExportIssues.xlsx
+++ b/Importexcel/wwwroot/ExportIssues.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>ease_import_sheet</t>
   </si>
@@ -173,28 +173,25 @@
     <t>1-11-2018 12:10:00</t>
   </si>
   <si>
-    <t>Hisham</t>
-  </si>
-  <si>
-    <t>Freeze</t>
-  </si>
-  <si>
-    <t>Browser Loopt vast</t>
-  </si>
-  <si>
-    <t>bekende bug , wordt opgelost</t>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>pagina crashed</t>
+  </si>
+  <si>
+    <t>word aan gewerkt</t>
+  </si>
+  <si>
+    <t>Geen haast</t>
   </si>
   <si>
     <t>Dave</t>
   </si>
   <si>
-    <t>3-11-2018 08:15:00</t>
-  </si>
-  <si>
-    <t>2-11-2018 09:45:00</t>
-  </si>
-  <si>
-    <t>2-11-2018 12:10:00</t>
+    <t>4-11-2018 00:00:00</t>
+  </si>
+  <si>
+    <t>3-11-2018 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -403,7 +400,7 @@
         <v>32</v>
       </c>
       <c r="S4" s="0">
-        <v>1098</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="5">
@@ -462,7 +459,7 @@
         <v>44</v>
       </c>
       <c r="S5" s="0">
-        <v>1099</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="6">
@@ -521,24 +518,24 @@
         <v>32</v>
       </c>
       <c r="S6" s="0">
-        <v>1100</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C7" s="0">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0">
-        <v>416</v>
+        <v>3</v>
       </c>
       <c r="E7" s="0">
-        <v>4153</v>
+        <v>4</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>45</v>
@@ -550,22 +547,22 @@
         <v>23</v>
       </c>
       <c r="I7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="K7" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="L7" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>57</v>
       </c>
       <c r="N7" s="0">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>58</v>
@@ -574,13 +571,13 @@
         <v>59</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="S7" s="0">
-        <v>1101</v>
+        <v>1166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>